<commit_message>
hongtong.liu: update version and scope doc
</commit_message>
<xml_diff>
--- a/第二组评审-图书管理系统项目评审意见处理.xlsx
+++ b/第二组评审-图书管理系统项目评审意见处理.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\北大\周三晚，软件需求工程\作业\software_requirement_work\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8535"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>图书管理系统项目评审表</t>
   </si>
@@ -423,6 +418,21 @@
 优先级已经在第8章需求分级中给出了。
 可以区分Actor。</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>列表的形式列举所有主要特性</t>
+  </si>
+  <si>
+    <t>刘洪通</t>
+  </si>
+  <si>
+    <t>暂时无法给出具体同时访问用户数。</t>
+  </si>
+  <si>
+    <t>有待确认</t>
+  </si>
+  <si>
+    <t>多字符集的支持正是为了达到一定的兼容性，尽可能避免乱码。</t>
   </si>
 </sst>
 </file>
@@ -599,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -704,6 +714,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,9 +742,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1011,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1336,9 +1361,15 @@
       <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="E18" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="21"/>
@@ -1351,9 +1382,15 @@
       <c r="D19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="E19" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="21"/>
@@ -1728,9 +1765,15 @@
       <c r="D40" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="E40" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="F40" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="G40" s="41" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="98.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="24"/>

</xml_diff>

<commit_message>
anbo.kang: update review excel
</commit_message>
<xml_diff>
--- a/第二组评审-图书管理系统项目评审意见处理.xlsx
+++ b/第二组评审-图书管理系统项目评审意见处理.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="137">
   <si>
     <t>图书管理系统项目评审表</t>
   </si>
@@ -433,6 +433,25 @@
   </si>
   <si>
     <t>多字符集的支持正是为了达到一定的兼容性，尽可能避免乱码。</t>
+  </si>
+  <si>
+    <t>康安博</t>
+  </si>
+  <si>
+    <t>这是我们的工作上的疏忽，下次会尽量避免</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是我们之前多为考虑到的，已进行补充完善</t>
+  </si>
+  <si>
+    <t>需增加的已进行增加，重新划分目录</t>
+  </si>
+  <si>
+    <t>这个是我们之前处理不到位，解释不清楚，以进行补充，解释</t>
+  </si>
+  <si>
+    <t>3.2与7内容看似相似，但是7里提到了3.2中所没有涉及的部分，如：系统易安装维护等特点是3.2里所没有涉及的，所以是否删有待商定</t>
   </si>
 </sst>
 </file>
@@ -609,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -664,6 +683,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -715,23 +752,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1036,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:G40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1052,28 +1086,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1083,14 +1117,14 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
       <c r="H3" s="6"/>
       <c r="I3" s="18" t="s">
         <v>6</v>
@@ -1124,7 +1158,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1136,12 +1170,18 @@
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="E5" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="21"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +1196,7 @@
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="21"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1171,7 +1211,7 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="21"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1186,7 +1226,7 @@
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="21"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1201,7 +1241,7 @@
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="21"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
@@ -1216,7 +1256,7 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="21"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1231,7 +1271,7 @@
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:9" ht="95.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="21"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1252,7 +1292,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="92.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1273,7 +1313,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="90.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1294,7 +1334,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1315,7 +1355,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="21"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="2" t="s">
         <v>47</v>
       </c>
@@ -1325,12 +1365,18 @@
       <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="E16" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="176.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="21"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1351,7 +1397,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
@@ -1361,18 +1407,18 @@
       <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="20" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="21"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
@@ -1382,18 +1428,18 @@
       <c r="D19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="22" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="21"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="2" t="s">
         <v>56</v>
       </c>
@@ -1408,7 +1454,7 @@
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="108" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="21"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
@@ -1429,7 +1475,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="65.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="21"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="2" t="s">
         <v>62</v>
       </c>
@@ -1444,7 +1490,7 @@
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1453,7 +1499,7 @@
       <c r="C23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E23" s="13" t="s">
@@ -1467,14 +1513,14 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="21"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="13" t="s">
         <v>117</v>
       </c>
@@ -1486,14 +1532,14 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="22"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="13" t="s">
         <v>118</v>
       </c>
@@ -1505,7 +1551,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="26" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1514,7 +1560,7 @@
       <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="27"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="2" t="s">
         <v>75</v>
       </c>
@@ -1526,27 +1572,27 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="21"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="27"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="13"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="22"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="27"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="12" t="s">
         <v>80</v>
       </c>
@@ -1558,7 +1604,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="26" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1567,7 +1613,7 @@
       <c r="C29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="27"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="13" t="s">
         <v>119</v>
       </c>
@@ -1579,14 +1625,14 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="21"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="27"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="13" t="s">
         <v>123</v>
       </c>
@@ -1598,14 +1644,14 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="21"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="13" t="s">
         <v>122</v>
       </c>
@@ -1617,14 +1663,14 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="21"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="27"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="13" t="s">
         <v>124</v>
       </c>
@@ -1636,14 +1682,14 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="21"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="27"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="13" t="s">
         <v>120</v>
       </c>
@@ -1651,7 +1697,7 @@
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7" ht="132" x14ac:dyDescent="0.15">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="29" t="s">
         <v>89</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1663,12 +1709,18 @@
       <c r="D34" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="E34" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="24"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="2" t="s">
         <v>93</v>
       </c>
@@ -1689,7 +1741,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="24"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="2" t="s">
         <v>97</v>
       </c>
@@ -1710,7 +1762,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="24"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="2" t="s">
         <v>100</v>
       </c>
@@ -1725,7 +1777,7 @@
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="24"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="2" t="s">
         <v>102</v>
       </c>
@@ -1740,7 +1792,7 @@
       <c r="G38" s="12"/>
     </row>
     <row r="39" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="24"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="2" t="s">
         <v>104</v>
       </c>
@@ -1755,7 +1807,7 @@
       <c r="G39" s="12"/>
     </row>
     <row r="40" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="24"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="2" t="s">
         <v>106</v>
       </c>
@@ -1765,18 +1817,18 @@
       <c r="D40" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="F40" s="41" t="s">
+      <c r="F40" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G40" s="41" t="s">
+      <c r="G40" s="24" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="98.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="24"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="2" t="s">
         <v>108</v>
       </c>
@@ -1786,12 +1838,18 @@
       <c r="D41" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+      <c r="E41" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="24"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="15" t="s">
         <v>110</v>
       </c>
@@ -1801,12 +1859,18 @@
       <c r="D42" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="E42" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="24"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="15" t="s">
         <v>113</v>
       </c>
@@ -1821,7 +1885,7 @@
       <c r="G43" s="12"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="25"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="15" t="s">
         <v>115</v>
       </c>

</xml_diff>